<commit_message>
New Document test data
</commit_message>
<xml_diff>
--- a/Falcrum_Trunk/src/com/proj/suiteDOCS/testdata/DocumentsTestData.xlsx
+++ b/Falcrum_Trunk/src/com/proj/suiteDOCS/testdata/DocumentsTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeapThoughtProjectWS\Falcrum_Trunk\src\com\proj\suiteDOCS\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIWS\Falcrum_Trunk\src\com\proj\suiteDOCS\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,60 +19,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>To</t>
-  </si>
-  <si>
-    <t>CC</t>
-  </si>
-  <si>
-    <t>Shaik Khaleel</t>
-  </si>
-  <si>
-    <t>Subject</t>
-  </si>
-  <si>
-    <t>IsConfidential</t>
-  </si>
-  <si>
-    <t>ReasonForIssue</t>
-  </si>
-  <si>
-    <t>Issue for Action</t>
-  </si>
-  <si>
-    <t>Contract</t>
-  </si>
-  <si>
-    <t>Message</t>
-  </si>
-  <si>
-    <t>Message for New transmittal</t>
-  </si>
-  <si>
-    <t>New Transmittal from Automation</t>
-  </si>
-  <si>
-    <t>Anupama D. Thumrugoti</t>
-  </si>
-  <si>
-    <t>TxType</t>
-  </si>
-  <si>
-    <t>UnTick</t>
-  </si>
-  <si>
-    <t>Action-Level2</t>
-  </si>
-  <si>
-    <t>ForwardTo</t>
-  </si>
-  <si>
-    <t>Action-Level3</t>
-  </si>
-  <si>
-    <t>Correspondence</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>Choose a file</t>
+  </si>
+  <si>
+    <t>Documents_browse_testdata.docx</t>
+  </si>
+  <si>
+    <t>Destination Folder</t>
+  </si>
+  <si>
+    <t>Version Comments</t>
+  </si>
+  <si>
+    <t>Comments entered through automation while uploading document</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Document from Automation</t>
   </si>
 </sst>
 </file>
@@ -124,10 +91,9 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,85 +440,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.42578125" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
-    <col min="8" max="8" width="35.7109375" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" customWidth="1"/>
-    <col min="10" max="10" width="24.85546875" customWidth="1"/>
-    <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="13" max="13" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
       <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" t="s">
         <v>6</v>
-      </c>
-      <c r="G2" s="2"/>
-      <c r="H2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>